<commit_message>
prepare for git upload
finalize inputs and delete temp files
</commit_message>
<xml_diff>
--- a/outputs/2_dists_by_taxcode_proc_kendall.xlsx
+++ b/outputs/2_dists_by_taxcode_proc_kendall.xlsx
@@ -919,10 +919,10 @@
     <t xml:space="preserve">H 101; H 111; H 18</t>
   </si>
   <si>
-    <t xml:space="preserve">C B PHILLIPS PUB LBRY DIST; OSWEGO LBRY DIST; PLAINFIELD LBRY DIST; PLANO COMM LBRY DIST; SANDWICH PUB LBRY DIST; THREE RIVERS LBRY DIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AURORA LIBRARY; JOLIET PUBLIC LIBRARY; YORKVILLE LIBRARY</t>
+    <t xml:space="preserve">AURORA LIBRARY; C B PHILLIPS PUB LBRY DIST; OSWEGO LBRY DIST; PLAINFIELD LBRY DIST; PLANO COMM LBRY DIST; SANDWICH PUB LBRY DIST; THREE RIVERS LBRY DIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOLIET PUBLIC LIBRARY; YORKVILLE LIBRARY</t>
   </si>
   <si>
     <t xml:space="preserve">AURORA; JOLIET; LISBON; MILLBROOK; MILLINGTON; MINOOKA; MONTGOMERY; NEWARK; OSWEGO; PLAINFIELD; PLANO; PLATTVILLE; SANDWICH; YORKVILLE</t>
@@ -7791,11 +7791,11 @@
         <v>24</v>
       </c>
       <c r="G156"/>
-      <c r="H156"/>
+      <c r="H156" t="s">
+        <v>258</v>
+      </c>
       <c r="I156"/>
-      <c r="J156" t="s">
-        <v>258</v>
-      </c>
+      <c r="J156"/>
       <c r="K156" t="s">
         <v>259</v>
       </c>
@@ -7836,11 +7836,11 @@
         <v>24</v>
       </c>
       <c r="G157"/>
-      <c r="H157"/>
+      <c r="H157" t="s">
+        <v>258</v>
+      </c>
       <c r="I157"/>
-      <c r="J157" t="s">
-        <v>258</v>
-      </c>
+      <c r="J157"/>
       <c r="K157" t="s">
         <v>259</v>
       </c>
@@ -7877,11 +7877,11 @@
         <v>24</v>
       </c>
       <c r="G158"/>
-      <c r="H158"/>
+      <c r="H158" t="s">
+        <v>258</v>
+      </c>
       <c r="I158"/>
-      <c r="J158" t="s">
-        <v>258</v>
-      </c>
+      <c r="J158"/>
       <c r="K158" t="s">
         <v>259</v>
       </c>
@@ -8088,11 +8088,11 @@
         <v>24</v>
       </c>
       <c r="G163"/>
-      <c r="H163"/>
+      <c r="H163" t="s">
+        <v>258</v>
+      </c>
       <c r="I163"/>
-      <c r="J163" t="s">
-        <v>258</v>
-      </c>
+      <c r="J163"/>
       <c r="K163" t="s">
         <v>259</v>
       </c>

</xml_diff>